<commit_message>
247around invoice templates fixed
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/247around_Tax_Invoice_Inter State.xlsx
+++ b/application/controllers/excel-templates/247around_Tax_Invoice_Inter State.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tax Invoice - Inter State" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>Invoice Date: {meta:invoice_date}</t>
   </si>
   <si>
-    <t>Service Period: {meta:sd} - {meta:ed}</t>
-  </si>
-  <si>
     <t>Reverse Charge (Y/N):</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>Total Amt after Tax</t>
+  </si>
+  <si>
+    <t>Period: {meta:sd} - {meta:ed}</t>
   </si>
 </sst>
 </file>
@@ -1059,89 +1059,76 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1156,39 +1143,45 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1201,95 +1194,102 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1686,8 +1686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10:Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1733,70 +1733,70 @@
     </row>
     <row r="2" spans="1:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="44"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="61"/>
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="46"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="71" t="s">
+      <c r="F3" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="72" t="s">
-        <v>50</v>
-      </c>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="47"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="67"/>
       <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="46"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="63"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
-      <c r="G4" s="66" t="s">
+      <c r="G4" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
       <c r="N4" s="13"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="47"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="67"/>
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -1806,15 +1806,15 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
       <c r="P5" s="9"/>
@@ -1823,605 +1823,605 @@
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="77" t="s">
+      <c r="B6" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="57"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="71"/>
+      <c r="N6" s="71"/>
+      <c r="O6" s="71"/>
+      <c r="P6" s="71"/>
+      <c r="Q6" s="72"/>
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:18" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="78"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="79"/>
-      <c r="M7" s="79"/>
-      <c r="N7" s="79"/>
-      <c r="O7" s="79"/>
-      <c r="P7" s="79"/>
-      <c r="Q7" s="80"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="75"/>
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="76" t="s">
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="74"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="74"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="74"/>
-      <c r="P8" s="74"/>
-      <c r="Q8" s="75"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="38"/>
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="76" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" s="74"/>
-      <c r="L9" s="74"/>
-      <c r="M9" s="74"/>
-      <c r="N9" s="74"/>
-      <c r="O9" s="74"/>
-      <c r="P9" s="74"/>
-      <c r="Q9" s="75"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="69" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="38"/>
       <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="85" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="83"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="84"/>
+      <c r="J10" s="77"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="78"/>
+      <c r="N10" s="78"/>
+      <c r="O10" s="78"/>
+      <c r="P10" s="78"/>
+      <c r="Q10" s="79"/>
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="95" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="40"/>
-      <c r="O11" s="40"/>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="96"/>
+      <c r="B11" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="46"/>
+      <c r="Q11" s="47"/>
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="90" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
-      <c r="L12" s="74"/>
-      <c r="M12" s="74"/>
-      <c r="N12" s="74"/>
-      <c r="O12" s="74"/>
-      <c r="P12" s="74"/>
-      <c r="Q12" s="75"/>
+      <c r="B12" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="38"/>
       <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="91" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="92"/>
-      <c r="D13" s="92"/>
-      <c r="E13" s="92"/>
-      <c r="F13" s="92"/>
-      <c r="G13" s="92"/>
-      <c r="H13" s="92"/>
-      <c r="I13" s="92"/>
-      <c r="J13" s="92"/>
-      <c r="K13" s="92"/>
-      <c r="L13" s="92"/>
-      <c r="M13" s="92"/>
-      <c r="N13" s="92"/>
-      <c r="O13" s="92"/>
-      <c r="P13" s="92"/>
-      <c r="Q13" s="82"/>
+      <c r="B13" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="41"/>
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:18" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="93"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="94"/>
-      <c r="J14" s="94"/>
-      <c r="K14" s="94"/>
-      <c r="L14" s="94"/>
-      <c r="M14" s="94"/>
-      <c r="N14" s="94"/>
-      <c r="O14" s="94"/>
-      <c r="P14" s="94"/>
-      <c r="Q14" s="26"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="44"/>
       <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="97" t="s">
+      <c r="B15" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="98"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
-      <c r="G15" s="98"/>
-      <c r="H15" s="98"/>
-      <c r="I15" s="98" t="s">
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="J15" s="98"/>
-      <c r="K15" s="98"/>
-      <c r="L15" s="98"/>
-      <c r="M15" s="98"/>
-      <c r="N15" s="98"/>
-      <c r="O15" s="99"/>
-      <c r="P15" s="81" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q15" s="82"/>
+      <c r="Q15" s="41"/>
       <c r="R15" s="2"/>
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="B16" s="104" t="s">
+      <c r="B16" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="106"/>
-      <c r="H16" s="110" t="s">
+      <c r="I16" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I16" s="110" t="s">
+      <c r="J16" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="110" t="s">
+      <c r="K16" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="100" t="s">
+      <c r="L16" s="21"/>
+      <c r="M16" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="101"/>
-      <c r="M16" s="85" t="s">
+      <c r="N16" s="81"/>
+      <c r="O16" s="82"/>
+      <c r="P16" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="N16" s="86"/>
-      <c r="O16" s="87"/>
-      <c r="P16" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q16" s="63"/>
+      <c r="Q16" s="52"/>
       <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="107"/>
-      <c r="C17" s="108"/>
-      <c r="D17" s="108"/>
-      <c r="E17" s="108"/>
-      <c r="F17" s="108"/>
-      <c r="G17" s="109"/>
-      <c r="H17" s="111"/>
-      <c r="I17" s="111"/>
-      <c r="J17" s="111"/>
-      <c r="K17" s="102"/>
-      <c r="L17" s="103"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="23"/>
       <c r="M17" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="N17" s="88" t="s">
-        <v>24</v>
-      </c>
-      <c r="O17" s="89"/>
-      <c r="P17" s="64"/>
-      <c r="Q17" s="65"/>
+        <v>19</v>
+      </c>
+      <c r="N17" s="83" t="s">
+        <v>23</v>
+      </c>
+      <c r="O17" s="84"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="54"/>
       <c r="R17" s="2"/>
     </row>
     <row r="18" spans="1:18" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
-      <c r="B18" s="112" t="s">
+      <c r="B18" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="113"/>
-      <c r="D18" s="113"/>
-      <c r="E18" s="113"/>
-      <c r="F18" s="113"/>
-      <c r="G18" s="114"/>
-      <c r="H18" s="115" t="s">
+      <c r="I18" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="116" t="s">
+      <c r="J18" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="J18" s="115" t="s">
+      <c r="K18" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="K18" s="117" t="s">
+      <c r="L18" s="32"/>
+      <c r="M18" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="L18" s="114"/>
-      <c r="M18" s="115" t="s">
+      <c r="N18" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="N18" s="117" t="s">
+      <c r="O18" s="32"/>
+      <c r="P18" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="O18" s="114"/>
-      <c r="P18" s="117" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q18" s="118"/>
+      <c r="Q18" s="113"/>
       <c r="R18" s="11"/>
     </row>
     <row r="19" spans="1:18" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="126" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="127"/>
       <c r="D19" s="127"/>
       <c r="E19" s="127"/>
       <c r="F19" s="127"/>
       <c r="G19" s="128"/>
-      <c r="H19" s="129"/>
-      <c r="I19" s="130" t="s">
+      <c r="H19" s="18"/>
+      <c r="I19" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" s="19"/>
+      <c r="K19" s="124" t="s">
         <v>33</v>
       </c>
-      <c r="J19" s="130"/>
-      <c r="K19" s="131" t="s">
+      <c r="L19" s="125"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="L19" s="132"/>
-      <c r="M19" s="130"/>
-      <c r="N19" s="131" t="s">
+      <c r="O19" s="125"/>
+      <c r="P19" s="124" t="s">
         <v>35</v>
-      </c>
-      <c r="O19" s="132"/>
-      <c r="P19" s="131" t="s">
-        <v>36</v>
       </c>
       <c r="Q19" s="133"/>
       <c r="R19" s="2"/>
     </row>
     <row r="20" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="119" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="120"/>
-      <c r="D20" s="120"/>
-      <c r="E20" s="120"/>
-      <c r="F20" s="120"/>
-      <c r="G20" s="120"/>
-      <c r="H20" s="120"/>
-      <c r="I20" s="120"/>
-      <c r="J20" s="120"/>
+      <c r="B20" s="129" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="130"/>
+      <c r="D20" s="130"/>
+      <c r="E20" s="130"/>
+      <c r="F20" s="130"/>
+      <c r="G20" s="130"/>
+      <c r="H20" s="130"/>
+      <c r="I20" s="130"/>
+      <c r="J20" s="130"/>
       <c r="K20" s="121" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L20" s="122"/>
       <c r="M20" s="122"/>
       <c r="N20" s="122"/>
       <c r="O20" s="123"/>
-      <c r="P20" s="124" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q20" s="125"/>
+      <c r="P20" s="131" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q20" s="132"/>
       <c r="R20" s="2"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="107" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="108"/>
+      <c r="D21" s="108"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="108"/>
+      <c r="G21" s="108"/>
+      <c r="H21" s="108"/>
+      <c r="I21" s="108"/>
+      <c r="J21" s="109"/>
+      <c r="K21" s="114" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="27" t="s">
+      <c r="L21" s="115"/>
+      <c r="M21" s="115"/>
+      <c r="N21" s="115"/>
+      <c r="O21" s="116"/>
+      <c r="P21" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="29"/>
-      <c r="P21" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q21" s="34"/>
+      <c r="Q21" s="118"/>
       <c r="R21" s="2"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q22" s="36"/>
+      <c r="B22" s="110"/>
+      <c r="C22" s="111"/>
+      <c r="D22" s="111"/>
+      <c r="E22" s="111"/>
+      <c r="F22" s="111"/>
+      <c r="G22" s="111"/>
+      <c r="H22" s="111"/>
+      <c r="I22" s="111"/>
+      <c r="J22" s="112"/>
+      <c r="K22" s="86" t="s">
+        <v>51</v>
+      </c>
+      <c r="L22" s="87"/>
+      <c r="M22" s="87"/>
+      <c r="N22" s="87"/>
+      <c r="O22" s="88"/>
+      <c r="P22" s="119" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q22" s="120"/>
       <c r="R22" s="2"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="106" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="102"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="61"/>
+      <c r="K23" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="L23" s="51"/>
-      <c r="M23" s="51"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="52"/>
-      <c r="P23" s="53">
+      <c r="L23" s="93"/>
+      <c r="M23" s="93"/>
+      <c r="N23" s="93"/>
+      <c r="O23" s="94"/>
+      <c r="P23" s="95">
         <f>IF(I10="Y",P21,0)</f>
         <v>0</v>
       </c>
-      <c r="Q23" s="54"/>
+      <c r="Q23" s="96"/>
       <c r="R23" s="2"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="104"/>
+      <c r="D24" s="104"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="104"/>
+      <c r="G24" s="105"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="63"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="56" t="s">
-        <v>46</v>
-      </c>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="57"/>
+      <c r="L24" s="71"/>
+      <c r="M24" s="71"/>
+      <c r="N24" s="71"/>
+      <c r="O24" s="71"/>
+      <c r="P24" s="71"/>
+      <c r="Q24" s="72"/>
       <c r="R24" s="2"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="47"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="59"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="59"/>
-      <c r="Q25" s="60"/>
+      <c r="B25" s="86" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="87"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="88"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="63"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="99"/>
+      <c r="L25" s="100"/>
+      <c r="M25" s="100"/>
+      <c r="N25" s="100"/>
+      <c r="O25" s="100"/>
+      <c r="P25" s="100"/>
+      <c r="Q25" s="101"/>
       <c r="R25" s="2"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
-      <c r="B26" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="61"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="43"/>
-      <c r="O26" s="43"/>
-      <c r="P26" s="43"/>
-      <c r="Q26" s="44"/>
+      <c r="B26" s="86" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="87"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="88"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="63"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="102"/>
+      <c r="L26" s="60"/>
+      <c r="M26" s="60"/>
+      <c r="N26" s="60"/>
+      <c r="O26" s="60"/>
+      <c r="P26" s="60"/>
+      <c r="Q26" s="61"/>
       <c r="R26" s="2"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="47"/>
-      <c r="K27" s="45"/>
-      <c r="L27" s="46"/>
-      <c r="M27" s="46"/>
-      <c r="N27" s="46"/>
-      <c r="O27" s="46"/>
-      <c r="P27" s="46"/>
-      <c r="Q27" s="47"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="63"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="63"/>
+      <c r="P27" s="63"/>
+      <c r="Q27" s="67"/>
       <c r="R27" s="2"/>
     </row>
     <row r="28" spans="1:18" ht="4" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="B28" s="45"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="46"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="46"/>
-      <c r="M28" s="46"/>
-      <c r="N28" s="46"/>
-      <c r="O28" s="46"/>
-      <c r="P28" s="46"/>
-      <c r="Q28" s="47"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="63"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="64"/>
+      <c r="L28" s="63"/>
+      <c r="M28" s="63"/>
+      <c r="N28" s="63"/>
+      <c r="O28" s="63"/>
+      <c r="P28" s="63"/>
+      <c r="Q28" s="67"/>
       <c r="R28" s="2"/>
     </row>
     <row r="29" spans="1:18" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="45"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="48"/>
-      <c r="L29" s="49"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="49"/>
-      <c r="O29" s="49"/>
-      <c r="P29" s="49"/>
-      <c r="Q29" s="41"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="63"/>
+      <c r="J29" s="67"/>
+      <c r="K29" s="90"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="58"/>
+      <c r="N29" s="58"/>
+      <c r="O29" s="58"/>
+      <c r="P29" s="58"/>
+      <c r="Q29" s="91"/>
       <c r="R29" s="2"/>
     </row>
     <row r="30" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="L30" s="49"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="49"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="49"/>
-      <c r="Q30" s="41"/>
+      <c r="B30" s="90"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="91"/>
+      <c r="H30" s="90"/>
+      <c r="I30" s="58"/>
+      <c r="J30" s="91"/>
+      <c r="K30" s="97" t="s">
+        <v>48</v>
+      </c>
+      <c r="L30" s="58"/>
+      <c r="M30" s="58"/>
+      <c r="N30" s="58"/>
+      <c r="O30" s="58"/>
+      <c r="P30" s="58"/>
+      <c r="Q30" s="91"/>
       <c r="R30" s="2"/>
     </row>
     <row r="31" spans="1:18" ht="4" customHeight="1" x14ac:dyDescent="0.2">
@@ -2446,18 +2446,32 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="K16:L17"/>
-    <mergeCell ref="B16:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="B12:Q12"/>
-    <mergeCell ref="B13:Q14"/>
-    <mergeCell ref="B11:Q11"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="I15:O15"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B21:J22"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="K21:O21"/>
+    <mergeCell ref="K22:O22"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="K20:O20"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G30"/>
+    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="K30:Q30"/>
+    <mergeCell ref="K24:Q25"/>
+    <mergeCell ref="K26:Q29"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="H23:J30"/>
     <mergeCell ref="P16:Q17"/>
     <mergeCell ref="G4:M4"/>
     <mergeCell ref="G5:M5"/>
@@ -2474,32 +2488,18 @@
     <mergeCell ref="N17:O17"/>
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="J9:Q9"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G30"/>
-    <mergeCell ref="K23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="K30:Q30"/>
-    <mergeCell ref="K24:Q25"/>
-    <mergeCell ref="K26:Q29"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="H23:J30"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B21:J22"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="K21:O21"/>
-    <mergeCell ref="K22:O22"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="K20:O20"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="B12:Q12"/>
+    <mergeCell ref="B13:Q14"/>
+    <mergeCell ref="B11:Q11"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="I15:O15"/>
+    <mergeCell ref="K16:L17"/>
+    <mergeCell ref="B16:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K18:L18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>